<commit_message>
Actualización Malla Abalisis Papers Sept 17 2019
</commit_message>
<xml_diff>
--- a/Articulo Estado Arte/Malla Analisis Papers.xlsx
+++ b/Articulo Estado Arte/Malla Analisis Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sin definir\Desktop\ModelosED\ModelosED\Articulo Estado Arte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF77E15-7615-4F6D-9C28-CCDEEDCAF31E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23683C67-84DD-4071-87C9-B7E7AD5043E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8685" xr2:uid="{97F21C58-349C-4EBA-9621-5722AD736A3E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Trabajo</t>
   </si>
@@ -264,6 +264,41 @@
     <t xml:space="preserve">Alessandro Vacca  and Italo Meloni (2013) Understanding route switch behavior: an analysis using GPS based
 data
 </t>
+  </si>
+  <si>
+    <t>..\..\..\..\Dropbox\Doctorado\Tesis Doctorado\ULTIMAS TAREAS\Articulos Borrador Articulo Revista\Tawfik, Rakha, Miller - 2010 - Driver route choice behavior Experiences, perceptions, and choices.pdf</t>
+  </si>
+  <si>
+    <t>la investigación presentada en este documento monitorea y analiza el comportamiento real de elección de ruta humana. Compara las experiencias, las percepciones y las elecciones reales de los conductores, y demuestra que (a) las percepciones de los conductores son significativamente diferentes de sus experiencias reales, y que las elecciones de los conductores se explican mejor por sus percepciones que por sus experiencias; (b) los conductores perciben las velocidades de viaje mejor que los tiempos de viaje (c) las velocidades de viaje percibidas parecen influir en la elección de ruta más que los tiempos de viaje percibidos, y (d) el comportamiento de elección de ruta de los conductores difiere entre los diferentes grupos de conductores.</t>
+  </si>
+  <si>
+    <t>A diferencia de la mayoría de las investigaciones de elección de ruta que se basan en suposiciones de comportamiento racional y se centran principalmente en el producto final de la elección de ruta, esta investigación intenta investigar la validez de estas suposiciones. Adicionalmente explora la precisión de las percepciones de los conductores y examina los motivos de la elección de ruta en función de las percepciones de los conductores las cuales se comparan con sus elecciones. En un intento de sopesar la fidelidad de las percepciones de los conductores, este trabajo también captura las experiencias reales de los conductores y las cruza o correlaciona con sus percepciones.
+Los objetivos de este estudio son demostrar que:
+(a) las percepciones de los conductores pueden ser significativamente diferentes de sus experiencias reales, y las elecciones de los conductores se explican mejor por sus percepciones que por sus experiencias;
+(b) los conductores pueden percibir las velocidades de viaje mejor que los tiempos de viaje
+(c) las velocidades de viaje percibidas parecen influir en la elección de ruta más que los tiempos de viaje percibidos, y
+  (d) el comportamiento de elección de ruta de los conductores difiere entre los diferentes grupos de conductores.</t>
+  </si>
+  <si>
+    <t>el experimento se realizó utilizando el software simulador de controlador STISIM desarrollado por Systems Technology Inc. (STI). STISIM Drive es un programa interactivo que es capaz de grabar numerosas medidas de rendimiento. El programa ofrece al investigador control sobre el desarrollo de escenarios de conducción, asegurando que todos los participantes se encuentren con los mismos eventos y condiciones mientras conducen. También ofrece al investigador una posible aleatorización parcial en el escenario y los eventos simulados. La investigación utilizó una red compuesta por dos rutas geométricamente idénticas con rutas casi idénticas (pero sesgadas estadísticamente), con tiempos de viaje promedio de 3 a 4 minutos con una velocidad promedio de aproximadamente 56 a 40 km / h (35 a 25 mph),
+El programa de conducción simulada funciona en una estructura similar al vehículo con un monitor de 48 cm (19 pulg.). La estructura similar al vehículo está equipada con una silla del vehículo, un volante y pedales de aceleración y freno.
+La investigación involucró a un total de cincuenta participantes. Se solicito llenar un cuestionario inicial antes de realizar las tareas de conducción el cual recolectó información sobre su edad, género, etnia, educación, problemas de visión, años de manejo y el número promedio de millas recorridas por año, despues de la actividad en el simulados se solicito a los participantes que rellenaran un breve cuestionarioel cual  fue diseñado para capturar la cognición de los participantes de las diferentes secciones de este estudio. El cuestionario recolectó información sobre sus percepciones de las diferencias en las características del viaje.</t>
+  </si>
+  <si>
+    <t>Ningun aporte</t>
+  </si>
+  <si>
+    <t>Se hizo fue un analisis estadistico sobre las actividades realizadas por los conductores y sobre las encuestas que cada uno al inicio y al final de la actividad entrego….</t>
+  </si>
+  <si>
+    <t>No usaron datos reales, solo datos y actividades sobre la conduccion que se realizaban el el simulador</t>
+  </si>
+  <si>
+    <t>No es claro</t>
+  </si>
+  <si>
+    <t>Tawfik, . Rakha and  Miller (2010) Driver Route Choice Behavior: Experiences, Perceptions, and
+Choices</t>
   </si>
 </sst>
 </file>
@@ -672,16 +707,16 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="97.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="93" style="1" customWidth="1"/>
+    <col min="4" max="4" width="103.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="61.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="82.28515625" style="1" customWidth="1"/>
@@ -937,17 +972,35 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+    <row r="10" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -1223,6 +1276,7 @@
     <hyperlink ref="J7" r:id="rId6" xr:uid="{C9A7BBF9-8A7A-4696-BEFA-45444DCFFA3E}"/>
     <hyperlink ref="J8" r:id="rId7" xr:uid="{59465331-82BA-4E53-9EDE-9DFE5FB27E99}"/>
     <hyperlink ref="J9" r:id="rId8" xr:uid="{90DEA886-25B7-4F55-8C5E-1C4330740EC8}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{6C722C3E-363C-49FE-805D-CCA41EE3F1F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>